<commit_message>
Minor fixes in top overlay
</commit_message>
<xml_diff>
--- a/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\AnalogIO-CAN-HW\Altium_prj\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\AnalogIO-CAN-HW\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB89FE78-9BD8-4A9C-926F-E9D628A0F7E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18C85EC8-DFE3-4190-B4AE-12F649AFBA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{B8D91EE1-2048-4A01-81B0-76899DBF7DE9}"/>
+    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{DB0EB517-D668-4590-8B1B-9E3A023D667F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CAN_CurrentLo" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,451 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>APP1, STS1</t>
+    <t>C1C1, C1C2, C1C3, C1C4</t>
+  </si>
+  <si>
+    <t>C0805C102J2GECAUTO</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>1 nF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 1 nF 200 V 5% Capacitor</t>
+  </si>
+  <si>
+    <t>CAP 0805_2012</t>
+  </si>
+  <si>
+    <t>C2C1, C2C2, C2C3, C2C4</t>
+  </si>
+  <si>
+    <t>C0805C103K5GEC7210</t>
+  </si>
+  <si>
+    <t>10 nF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 10 nF 50 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C3C1, C3C2, C3C3, C3C4, C18, C24, C26</t>
+  </si>
+  <si>
+    <t>08055C104K4Z2A, 0805YC104KAT4A</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 100 nF 50 V 10% Capacitor, MLCC Ceramic 100 nF 16 v 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C4, C11, C13, C15, C16, C17, C28, C29, C31, C34, C36</t>
+  </si>
+  <si>
+    <t>0603YC104KAT2A, 06035C104K4Z2A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 100 nF 16 V 10% Capacitor, MLCC Ceramic 100 nF 50 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>CAP 0603_1608</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C8</t>
+  </si>
+  <si>
+    <t>0603ZA102JAT4A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 1 nF 10 V 5% Capacitor</t>
+  </si>
+  <si>
+    <t>C9, C10</t>
+  </si>
+  <si>
+    <t>06035A6R8C4T4A</t>
+  </si>
+  <si>
+    <t>6.8 pF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 6.8 pF 50 V 0.25 pF Capacitor</t>
+  </si>
+  <si>
+    <t>C12, C33</t>
+  </si>
+  <si>
+    <t>0603YC105KAT2A, 06033C105KAT4A</t>
+  </si>
+  <si>
+    <t>1 uF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor, MLCC Ceramic 1 uF 25 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>GRM188Z71A475ME15D</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>4.7 uF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 4.7 uF 10 V 20% Capacitor</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>HHXA630ARA220MF80G</t>
+  </si>
+  <si>
+    <t>United Chemi-Con</t>
+  </si>
+  <si>
+    <t>22 uF</t>
+  </si>
+  <si>
+    <t>Aluminum Electrolytic 22 uF 63 V 20% Capacitor</t>
+  </si>
+  <si>
+    <t>CAP ALSMD 6.3MM H7.7MM</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>12065C225K4T2A</t>
+  </si>
+  <si>
+    <t>2.2 uF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 2.2 uF 50 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>CAP 1206_3216 - 1.8MM</t>
+  </si>
+  <si>
+    <t>C21, C22</t>
+  </si>
+  <si>
+    <t>1206YC106KAT2A</t>
+  </si>
+  <si>
+    <t>10 uF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 10 uF 16 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C23, C25, C27, C35</t>
+  </si>
+  <si>
+    <t>0805YC106MAT2A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 10 uF 25 V 20% Capacitor</t>
+  </si>
+  <si>
+    <t>C30, C32</t>
+  </si>
+  <si>
+    <t>0805YC105KAT4A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C37, C39</t>
+  </si>
+  <si>
+    <t>06031A680FAT2A</t>
+  </si>
+  <si>
+    <t>68 pF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 68 pF 100 V 1% Capacitor</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>06031U470FAT2A</t>
+  </si>
+  <si>
+    <t>47 pF</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 47 pF 100 V 1% Capacitor</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C0603C103J4GACTU</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 10 nF 16 V 5% Capacitor</t>
+  </si>
+  <si>
+    <t>D1C1, D1C2, D1C3, D1C4, D5C1, D5C2, D5C3, D5C4</t>
+  </si>
+  <si>
+    <t>BAT46JFILM</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>SOD323</t>
+  </si>
+  <si>
+    <t>D2C1, D2C2, D2C3, D2C4, D4C1, D4C2, D4C3, D4C4</t>
+  </si>
+  <si>
+    <t>CDSU101A-HF</t>
+  </si>
+  <si>
+    <t>Comchip Technology</t>
+  </si>
+  <si>
+    <t>General Purpose Diode</t>
+  </si>
+  <si>
+    <t>SOD523F</t>
+  </si>
+  <si>
+    <t>D3C1, D3C2, D3C3, D3C4</t>
+  </si>
+  <si>
+    <t>SM6T39CAY</t>
+  </si>
+  <si>
+    <t>TVS Diode</t>
+  </si>
+  <si>
+    <t>DO214AA SMB</t>
+  </si>
+  <si>
+    <t>D6C1, D6C2, D6C3, D6C4</t>
+  </si>
+  <si>
+    <t>BZX384C3V3-E3-08</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>Zener Diode 3.3 V 200 mW</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>MMSZ5240BS-7-F</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>Zener 200 mW 10 V</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>MBRA160</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>Schottky Rectifier Diode</t>
+  </si>
+  <si>
+    <t>DO214AC SMA</t>
+  </si>
+  <si>
+    <t>D9, D10</t>
+  </si>
+  <si>
+    <t>MBR0520L</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>CDSOT23-SM712</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>CAN bus TVS diode</t>
+  </si>
+  <si>
+    <t>BOURNS SOT-23-3</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>NANOASMDC012F-2</t>
+  </si>
+  <si>
+    <t>Littelfuse</t>
+  </si>
+  <si>
+    <t>PPTC .12A 48V Nano SMD AEC-Q200</t>
+  </si>
+  <si>
+    <t>PPTC_1206_1MM</t>
+  </si>
+  <si>
+    <t>FB1C1, FB1C2, FB1C3, FB1C4, FB2C1, FB2C2, FB2C3, FB2C4, FB3</t>
+  </si>
+  <si>
+    <t>BLM21SP601SH1D</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>600 Ohms</t>
+  </si>
+  <si>
+    <t>Ferrite bead</t>
+  </si>
+  <si>
+    <t>FER 0805_2012</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>ZXMP10A18GTA</t>
+  </si>
+  <si>
+    <t>MOSFET 100V P-Chnl UMOS</t>
+  </si>
+  <si>
+    <t>DIODES SOT-223</t>
+  </si>
+  <si>
+    <t>J1C1, J1C2, J1C3, J1C4, J3</t>
+  </si>
+  <si>
+    <t>1757475</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>Pluggable Terminal Blocks 2 Pos 5mm pitch Through Hole Header</t>
+  </si>
+  <si>
+    <t>MSTBA2</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>SHF-105-01-L-D-TH</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>Shrouded Terminal Strip, 0.050 pitch</t>
+  </si>
+  <si>
+    <t>SHF-105-01-X-D-TH</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>09681537613</t>
+  </si>
+  <si>
+    <t>Harting</t>
+  </si>
+  <si>
+    <t>DSUB SV FE SSDP ANG-US 09P AU3</t>
+  </si>
+  <si>
+    <t>DSUB9</t>
+  </si>
+  <si>
+    <t>JP1, JP2</t>
+  </si>
+  <si>
+    <t>61300211121</t>
+  </si>
+  <si>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 2 position 0.100 (2.54mm)</t>
+  </si>
+  <si>
+    <t>JUMPER-100</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>SRR1210-680M</t>
+  </si>
+  <si>
+    <t>68 uH</t>
+  </si>
+  <si>
+    <t>Shielded SMD Power Inductor 68 uH 3 A</t>
+  </si>
+  <si>
+    <t>SRR1210</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>ACT45B-510-2P-TL003</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>51 uH</t>
+  </si>
+  <si>
+    <t>CAN Bus Common Choke</t>
+  </si>
+  <si>
+    <t>TDK_ACT45B</t>
+  </si>
+  <si>
+    <t>LED1, LED2</t>
   </si>
   <si>
     <t>APTD1608LZGCK</t>
@@ -66,313 +510,7 @@
     <t>LED 0603_1608 GREEN</t>
   </si>
   <si>
-    <t>C1C1, C1C2, C1C3, C1C4</t>
-  </si>
-  <si>
-    <t>C0805C102J2GECAUTO</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>1 nF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 1 nF 200 V 5% Capacitor</t>
-  </si>
-  <si>
-    <t>CAP 0805_2012</t>
-  </si>
-  <si>
-    <t>C2C1, C2C2, C2C3, C2C4</t>
-  </si>
-  <si>
-    <t>C0805C103K5GEC7210</t>
-  </si>
-  <si>
-    <t>10 nF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 10 nF 50 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C3C1, C3C2, C3C3, C3C4, C18, C24, C26</t>
-  </si>
-  <si>
-    <t>08055C104K4Z2A, 0805YC104KAT4A</t>
-  </si>
-  <si>
-    <t>AVX</t>
-  </si>
-  <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 100 nF 50 V 10% Capacitor, MLCC Ceramic 100 nF 16 v 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C4, C11, C13, C15, C16, C17, C28, C29, C31, C34, C36</t>
-  </si>
-  <si>
-    <t>0603YC104KAT2A, 06035C104K4Z2A</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 100 nF 16 V 10% Capacitor, MLCC Ceramic 100 nF 50 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>CAP 0603_1608</t>
-  </si>
-  <si>
-    <t>C5, C6, C7, C8</t>
-  </si>
-  <si>
-    <t>0603ZA102JAT4A</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 1 nF 10 V 5% Capacitor</t>
-  </si>
-  <si>
-    <t>C9, C10</t>
-  </si>
-  <si>
-    <t>06035A6R8C4T4A</t>
-  </si>
-  <si>
-    <t>6.8 pF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 6.8 pF 50 V 0.25 pF Capacitor</t>
-  </si>
-  <si>
-    <t>C12, C33</t>
-  </si>
-  <si>
-    <t>0603YC105KAT2A, 06033C105KAT4A</t>
-  </si>
-  <si>
-    <t>1 uF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor, MLCC Ceramic 1 uF 25 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>GRM188Z71A475ME15D</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
-    <t>4.7 uF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 4.7 uF 10 V 20% Capacitor</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>HHXA630ARA220MF80G</t>
-  </si>
-  <si>
-    <t>United Chemi-Con</t>
-  </si>
-  <si>
-    <t>22 uF</t>
-  </si>
-  <si>
-    <t>Aluminum Electrolytic 22 uF 63 V 20% Capacitor</t>
-  </si>
-  <si>
-    <t>CAP ALSMD 6.3MM H7.7MM</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>12065C225K4T2A</t>
-  </si>
-  <si>
-    <t>2.2 uF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 2.2 uF 50 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>CAP 1206_3216 - 1.8MM</t>
-  </si>
-  <si>
-    <t>C21, C22</t>
-  </si>
-  <si>
-    <t>1206YC106KAT2A</t>
-  </si>
-  <si>
-    <t>10 uF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 10 uF 16 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C23, C25, C27, C35</t>
-  </si>
-  <si>
-    <t>0805YC106MAT2A</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 10 uF 25 V 20% Capacitor</t>
-  </si>
-  <si>
-    <t>C30, C32</t>
-  </si>
-  <si>
-    <t>0805YC105KAT4A</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C37, C39</t>
-  </si>
-  <si>
-    <t>06031A680FAT2A</t>
-  </si>
-  <si>
-    <t>68 pF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 68 pF 100 V 1% Capacitor</t>
-  </si>
-  <si>
-    <t>C38</t>
-  </si>
-  <si>
-    <t>06031U470FAT2A</t>
-  </si>
-  <si>
-    <t>47 pF</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 47 pF 100 V 1% Capacitor</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>C0603C103J4GACTU</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 10 nF 16 V 5% Capacitor</t>
-  </si>
-  <si>
-    <t>D1C1, D1C2, D1C3, D1C4, D5C1, D5C2, D5C3, D5C4</t>
-  </si>
-  <si>
-    <t>BAT46JFILM</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
-    <t>SOD323</t>
-  </si>
-  <si>
-    <t>D2C1, D2C2, D2C3, D2C4, D4C1, D4C2, D4C3, D4C4</t>
-  </si>
-  <si>
-    <t>CDSU101A-HF</t>
-  </si>
-  <si>
-    <t>Comchip Technology</t>
-  </si>
-  <si>
-    <t>General Purpose Diode</t>
-  </si>
-  <si>
-    <t>SOD523F</t>
-  </si>
-  <si>
-    <t>D3C1, D3C2, D3C3, D3C4</t>
-  </si>
-  <si>
-    <t>SM6T39CAY</t>
-  </si>
-  <si>
-    <t>TVS Diode</t>
-  </si>
-  <si>
-    <t>DO214AA SMB</t>
-  </si>
-  <si>
-    <t>D6C1, D6C2, D6C3, D6C4</t>
-  </si>
-  <si>
-    <t>BZX384C3V3-E3-08</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>Zener Diode 3.3 V 200 mW</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>MMSZ5240BS-7-F</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>Zener 200 mW 10 V</t>
-  </si>
-  <si>
-    <t>SOD-123</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>MBRA160</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>Schottky Rectifier Diode</t>
-  </si>
-  <si>
-    <t>DO214AC SMA</t>
-  </si>
-  <si>
-    <t>D9, D10</t>
-  </si>
-  <si>
-    <t>MBR0520L</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>CDSOT23-SM712</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>CAN bus TVS diode</t>
-  </si>
-  <si>
-    <t>BOURNS SOT-23-3</t>
-  </si>
-  <si>
-    <t>ERR1, PWR1</t>
+    <t>LED3, LED4</t>
   </si>
   <si>
     <t>APTD1608LSECK</t>
@@ -382,144 +520,6 @@
   </si>
   <si>
     <t>LED 0603_1608 RED</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>NANOASMDC012F-2</t>
-  </si>
-  <si>
-    <t>Littelfuse</t>
-  </si>
-  <si>
-    <t>PPTC .12A 48V Nano SMD AEC-Q200</t>
-  </si>
-  <si>
-    <t>PPTC_1206_1MM</t>
-  </si>
-  <si>
-    <t>FB1C1, FB1C2, FB1C3, FB1C4, FB2C1, FB2C2, FB2C3, FB2C4, FB3</t>
-  </si>
-  <si>
-    <t>BLM21SP601SH1D</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>600 Ohms</t>
-  </si>
-  <si>
-    <t>Ferrite bead</t>
-  </si>
-  <si>
-    <t>FER 0805_2012</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>ZXMP10A18GTA</t>
-  </si>
-  <si>
-    <t>MOSFET 100V P-Chnl UMOS</t>
-  </si>
-  <si>
-    <t>DIODES SOT-223</t>
-  </si>
-  <si>
-    <t>J1C1, J1C2, J1C3, J1C4, J3</t>
-  </si>
-  <si>
-    <t>1757475</t>
-  </si>
-  <si>
-    <t>Phoenix Contact</t>
-  </si>
-  <si>
-    <t>Pluggable Terminal Blocks 2 Pos 5mm pitch Through Hole Header</t>
-  </si>
-  <si>
-    <t>MSTBA2</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>SHF-105-01-L-D-TH</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>Shrouded Terminal Strip, 0.050 pitch</t>
-  </si>
-  <si>
-    <t>SHF-105-01-X-D-TH</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>09681537613</t>
-  </si>
-  <si>
-    <t>Harting</t>
-  </si>
-  <si>
-    <t>DSUB SV FE SSDP ANG-US 09P AU3</t>
-  </si>
-  <si>
-    <t>DSUB9</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>61300211121</t>
-  </si>
-  <si>
-    <t>Würth Elektronik</t>
-  </si>
-  <si>
-    <t>Connector Header Through Hole 2 position 0.100 (2.54mm)</t>
-  </si>
-  <si>
-    <t>JUMPER-100</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>SRR1210-680M</t>
-  </si>
-  <si>
-    <t>68 uH</t>
-  </si>
-  <si>
-    <t>Shielded SMD Power Inductor 68 uH 3 A</t>
-  </si>
-  <si>
-    <t>SRR1210</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>ACT45B-510-2P-TL003</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>51 uH</t>
-  </si>
-  <si>
-    <t>CAN Bus Common Choke</t>
-  </si>
-  <si>
-    <t>TDK_ACT45B</t>
   </si>
   <si>
     <t>Q1C1, Q1C2, Q1C3, Q1C4</t>
@@ -1204,7 +1204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236232F9-CC1B-486C-8E9A-83B0292ADB35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69504134-F454-4057-B719-0A82632F3478}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1257,27 +1257,27 @@
         <v>9</v>
       </c>
       <c r="D2" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4">
         <v>4</v>
@@ -1289,21 +1289,21 @@
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
@@ -1312,7 +1312,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1323,102 +1323,102 @@
         <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>40</v>
@@ -1427,7 +1427,7 @@
         <v>41</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1450,18 +1450,18 @@
         <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1484,10 +1484,10 @@
         <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>55</v>
@@ -1496,145 +1496,145 @@
         <v>56</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="4">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="4">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -1668,65 +1668,65 @@
         <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D20" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>91</v>
       </c>
       <c r="G21" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="4">
-        <v>4</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1760,45 +1760,45 @@
         <v>103</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D24" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>103</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="4">
-        <v>2</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>109</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>114</v>
       </c>
@@ -1829,59 +1829,59 @@
         <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="4">
         <v>9</v>
       </c>
-      <c r="D27" s="4">
-        <v>2</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="D29" s="4">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>127</v>
@@ -1890,7 +1890,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>129</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>130</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -1907,139 +1907,139 @@
         <v>130</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="4">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F32" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D34" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D35" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D36" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>161</v>
@@ -2082,7 +2082,7 @@
         <v>170</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D38" s="4">
         <v>4</v>
@@ -2174,7 +2174,7 @@
         <v>189</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D42" s="4">
         <v>4</v>
@@ -2335,7 +2335,7 @@
         <v>216</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -2427,7 +2427,7 @@
         <v>234</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -2606,6 +2606,6 @@
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="30" orientation="landscape" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="30" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed LDOs power connection to inner planes
</commit_message>
<xml_diff>
--- a/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\AnalogIO-CAN-HW\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18C85EC8-DFE3-4190-B4AE-12F649AFBA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA75C21A-CE78-4C0F-8135-30B81EF9E186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{DB0EB517-D668-4590-8B1B-9E3A023D667F}"/>
+    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{FC094E4E-D6E1-4A9F-BFC9-E89296C2195C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CAN_CurrentLo" sheetId="1" r:id="rId1"/>
@@ -1204,7 +1204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69504134-F454-4057-B719-0A82632F3478}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B982300-5615-4232-A95C-962619BF276E}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Fixed BOM format in order to group components only by their part number
</commit_message>
<xml_diff>
--- a/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\AnalogIO-CAN-HW\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA75C21A-CE78-4C0F-8135-30B81EF9E186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4313325-24A0-4590-BEF5-3706384D8689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{FC094E4E-D6E1-4A9F-BFC9-E89296C2195C}"/>
+    <workbookView xWindow="4320" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{C1A09651-E7C2-46C0-84B1-2A52B2150E59}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CAN_CurrentLo" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="272">
   <si>
     <t>Designator</t>
   </si>
@@ -81,10 +81,10 @@
     <t>MLCC Ceramic 10 nF 50 V 10% Capacitor</t>
   </si>
   <si>
-    <t>C3C1, C3C2, C3C3, C3C4, C18, C24, C26</t>
-  </si>
-  <si>
-    <t>08055C104K4Z2A, 0805YC104KAT4A</t>
+    <t>C3C1, C3C2, C3C3, C3C4, C18</t>
+  </si>
+  <si>
+    <t>08055C104K4Z2A</t>
   </si>
   <si>
     <t>AVX</t>
@@ -93,16 +93,16 @@
     <t>100 nF</t>
   </si>
   <si>
-    <t>MLCC Ceramic 100 nF 50 V 10% Capacitor, MLCC Ceramic 100 nF 16 v 10% Capacitor</t>
-  </si>
-  <si>
-    <t>C4, C11, C13, C15, C16, C17, C28, C29, C31, C34, C36</t>
-  </si>
-  <si>
-    <t>0603YC104KAT2A, 06035C104K4Z2A</t>
-  </si>
-  <si>
-    <t>MLCC Ceramic 100 nF 16 V 10% Capacitor, MLCC Ceramic 100 nF 50 V 10% Capacitor</t>
+    <t>MLCC Ceramic 100 nF 50 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C4, C11, C13, C15, C16, C17, C28, C29, C31, C34</t>
+  </si>
+  <si>
+    <t>0603YC104KAT2A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 100 nF 16 V 10% Capacitor</t>
   </si>
   <si>
     <t>CAP 0603_1608</t>
@@ -129,16 +129,16 @@
     <t>MLCC Ceramic 6.8 pF 50 V 0.25 pF Capacitor</t>
   </si>
   <si>
-    <t>C12, C33</t>
-  </si>
-  <si>
-    <t>0603YC105KAT2A, 06033C105KAT4A</t>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>0603YC105KAT2A</t>
   </si>
   <si>
     <t>1 uF</t>
   </si>
   <si>
-    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor, MLCC Ceramic 1 uF 25 V 10% Capacitor</t>
+    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor</t>
   </si>
   <si>
     <t>C14</t>
@@ -210,13 +210,34 @@
     <t>MLCC Ceramic 10 uF 25 V 20% Capacitor</t>
   </si>
   <si>
+    <t>C24, C26</t>
+  </si>
+  <si>
+    <t>0805YC104KAT4A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 100 nF 16 v 10% Capacitor</t>
+  </si>
+  <si>
     <t>C30, C32</t>
   </si>
   <si>
     <t>0805YC105KAT4A</t>
   </si>
   <si>
-    <t>MLCC Ceramic 1 uF 16 V 10% Capacitor</t>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>06033C105KAT4A</t>
+  </si>
+  <si>
+    <t>MLCC Ceramic 1 uF 25 V 10% Capacitor</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>06035C104K4Z2A</t>
   </si>
   <si>
     <t>C37, C39</t>
@@ -1204,11 +1225,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B982300-5615-4232-A95C-962619BF276E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CD1371-EA75-4821-A825-6D30F2324C07}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1220,7 +1241,7 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1292,7 +1313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1303,7 +1324,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
@@ -1326,7 +1347,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>20</v>
@@ -1384,7 +1405,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1395,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>35</v>
@@ -1536,7 +1557,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>62</v>
@@ -1559,21 +1580,21 @@
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
@@ -1582,10 +1603,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>25</v>
@@ -1593,1019 +1614,1088 @@
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="4">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="4">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="4">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="4">
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="4">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="4">
         <v>4</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="4">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="3" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="4">
+      <c r="B29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="4">
         <v>9</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="4">
-        <v>5</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="3" t="s">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D32" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D35" s="4">
         <v>2</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="4">
-        <v>2</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="4">
-        <v>4</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="4">
-        <v>4</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D39" s="4">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D40" s="4">
         <v>4</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D42" s="4">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="G42" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D43" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="4">
+        <v>4</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D46" s="4">
+        <v>6</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" s="4">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D47" s="4">
-        <v>2</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="G47" s="3" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D48" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D50" s="4">
+        <v>2</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G49" s="3" t="s">
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C51" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="4">
+        <v>3</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D50" s="4">
-        <v>4</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F50" s="3" t="s">
+      <c r="G51" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="C52" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D51" s="4">
-        <v>4</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D52" s="4">
-        <v>1</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="4">
+        <v>4</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="D54" s="4">
+        <v>4</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D53" s="4">
-        <v>1</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="F53" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="G53" s="3" t="s">
+    </row>
+    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C55" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="F54" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D55" s="4">
-        <v>1</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="4">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C57" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D56" s="4">
-        <v>1</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F56" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D57" s="4">
-        <v>2</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="C58" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" s="4">
-        <v>1</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D59" s="4">
         <v>1</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C61" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" s="4">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="3" t="s">
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="C62" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" s="4">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>264</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D63" s="4">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="30" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed some resistor values after testing REV1 board. Amplifier resistors has been changed to 56k instead of 63k in order to allow a less gain. Red LED resistor changed to cause brigthness is too low
</commit_message>
<xml_diff>
--- a/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -594,13 +594,13 @@
     <t>R5, R7, R9, R11</t>
   </si>
   <si>
-    <t>CRCW060362K0FKEAC</t>
-  </si>
-  <si>
-    <t>62 kOhms</t>
-  </si>
-  <si>
-    <t>Thin Film Resistor 62 kOhms 1%</t>
+    <t>CRCW060356K0FKEA</t>
+  </si>
+  <si>
+    <t>56 kOhms</t>
+  </si>
+  <si>
+    <t>Thin Film Resistor 56 kOhms 1%</t>
   </si>
   <si>
     <t>RES 0603_1608</t>
@@ -618,7 +618,7 @@
     <t>POT BOURNS TRIMPOT 3224W</t>
   </si>
   <si>
-    <t>R13, R14, R18, R24, R25, R26</t>
+    <t>R13, R14, R18, R24, R25</t>
   </si>
   <si>
     <t>CRCW060310K0FKEAC</t>
@@ -675,7 +675,7 @@
     <t>RES 1206_3216</t>
   </si>
   <si>
-    <t>R21, R22, R23</t>
+    <t>R21, R22, R23, R26</t>
   </si>
   <si>
     <t>CRCW06034K70FKEAC</t>
@@ -2225,7 +2225,7 @@
         <v>184</v>
       </c>
       <c r="D46" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" s="45" t="s">
         <v>185</v>
@@ -2340,7 +2340,7 @@
         <v>184</v>
       </c>
       <c r="D51" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" s="45" t="s">
         <v>221</v>

</xml_diff>

<commit_message>
Amplifier resistors has been changed to 60.4k instead of 56k in order to allow a less gain.
</commit_message>
<xml_diff>
--- a/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Fabrication/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -594,13 +594,13 @@
     <t>R5, R7, R9, R11</t>
   </si>
   <si>
-    <t>CRCW060356K0FKEA</t>
-  </si>
-  <si>
-    <t>56 kOhms</t>
-  </si>
-  <si>
-    <t>Thin Film Resistor 56 kOhms 1%</t>
+    <t>CRCW060360K4FKEA</t>
+  </si>
+  <si>
+    <t>60.4 kOhms</t>
+  </si>
+  <si>
+    <t>Thin Film Resistor 60.4 kOhms 1%</t>
   </si>
   <si>
     <t>RES 0603_1608</t>

</xml_diff>